<commit_message>
Atualização automática: Arquivo Excel modificado
</commit_message>
<xml_diff>
--- a/Resumo_Operacional_Com_Graficos.xlsx
+++ b/Resumo_Operacional_Com_Graficos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\Msacco IN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0FDFCB-AA9D-4305-A484-ACD85713F327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAF609B-73DD-417E-8AC1-829FC6F03B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4977,7 +4977,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5000,7 +5000,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="3">
-        <v>10</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5008,7 +5008,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="3">
-        <v>20</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5016,7 +5016,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="3">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5024,7 +5024,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3">
-        <v>40</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5032,7 +5032,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="3">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5040,7 +5040,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5048,7 +5048,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5056,7 +5056,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="3">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5064,7 +5064,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="3">
-        <v>90</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5072,7 +5072,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="3">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5080,7 +5080,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="3">
-        <v>110</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5088,7 +5088,7 @@
         <v>27</v>
       </c>
       <c r="B13" s="3">
-        <v>120</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Atualização automática pelo monitor.py
</commit_message>
<xml_diff>
--- a/Resumo_Operacional_Com_Graficos.xlsx
+++ b/Resumo_Operacional_Com_Graficos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\Msacco IN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4420EA0-A575-4613-AEE1-D3DE09341F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97E753F-E8A6-44CD-A099-4492701B3D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="34">
   <si>
     <t>Mês</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Total Despesas</t>
+  </si>
+  <si>
+    <t>Babi1312</t>
   </si>
 </sst>
 </file>
@@ -502,7 +505,7 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="A1:B13">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Mês"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Babi1312"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Total Despesas"/>
   </tableColumns>
   <tableStyleInfo name="Sheet2-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -6153,7 +6156,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6164,7 +6169,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>32</v>
@@ -6207,7 +6212,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="3">
-        <v>235</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>